<commit_message>
Fix funcao show no EquipmentController.php
</commit_message>
<xml_diff>
--- a/Documentation/Aulas Projeto.xlsx
+++ b/Documentation/Aulas Projeto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfernandes.PSCGROUP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\Projeto_Final\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1062BE-9F99-404D-960F-D14953F7963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274AA55E-D2B2-4187-B08E-0402DCF89487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C958B51-1073-4D1E-BDA4-5358410FDF66}"/>
   </bookViews>
@@ -179,9 +179,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -204,9 +201,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -214,6 +208,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,7 +533,7 @@
   <dimension ref="B8:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,586 +556,588 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="11" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="G8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="L8" s="11" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="L8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="Q8" s="11" t="s">
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="Q8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="T9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>44860</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>2</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="G10" s="7">
+      <c r="E10" s="12"/>
+      <c r="G10" s="6">
         <v>44837</v>
       </c>
-      <c r="H10" s="8">
-        <v>3</v>
-      </c>
-      <c r="I10" s="12">
-        <v>3</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="L10" s="3">
+      <c r="H10" s="7">
+        <v>3</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="L10" s="2">
         <v>44868</v>
       </c>
-      <c r="M10" s="4">
-        <v>3</v>
-      </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="14"/>
-      <c r="Q10" s="3">
+      <c r="M10" s="3">
+        <v>3</v>
+      </c>
+      <c r="N10" s="11"/>
+      <c r="O10" s="12"/>
+      <c r="Q10" s="2">
         <v>44897</v>
       </c>
-      <c r="R10" s="4">
-        <v>3</v>
-      </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="14"/>
+      <c r="R10" s="3">
+        <v>3</v>
+      </c>
+      <c r="S10" s="11"/>
+      <c r="T10" s="12"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="7">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="12"/>
+      <c r="G11" s="6">
         <v>44844</v>
       </c>
-      <c r="H11" s="8">
-        <v>3</v>
-      </c>
-      <c r="I11" s="8">
-        <v>3</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="L11" s="3">
+      <c r="H11" s="7">
+        <v>3</v>
+      </c>
+      <c r="I11" s="7">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="L11" s="2">
         <v>44869</v>
       </c>
-      <c r="M11" s="4">
-        <v>3</v>
-      </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="Q11" s="3">
+      <c r="M11" s="3">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="Q11" s="2">
         <v>44898</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <v>4</v>
       </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="14"/>
-      <c r="G12" s="3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="12"/>
+      <c r="G12" s="6">
         <v>44851</v>
       </c>
-      <c r="H12" s="4">
-        <v>3</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="L12" s="3">
+      <c r="H12" s="7">
+        <v>3</v>
+      </c>
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="L12" s="2">
         <v>44870</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>4</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="Q12" s="3">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="Q12" s="2">
         <v>44900</v>
       </c>
-      <c r="R12" s="4">
-        <v>3</v>
-      </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
+      <c r="R12" s="3">
+        <v>3</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="14"/>
-      <c r="G13" s="3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="12"/>
+      <c r="G13" s="2">
         <v>44854</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>2</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="L13" s="3">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="L13" s="2">
         <v>44872</v>
       </c>
-      <c r="M13" s="4">
-        <v>3</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="Q13" s="3">
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="Q13" s="2">
         <v>44902</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="3">
         <v>4</v>
       </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="12"/>
+      <c r="G14" s="2">
         <v>44856</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>2</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="L14" s="3">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="2">
         <v>44873</v>
       </c>
-      <c r="M14" s="4">
-        <v>3</v>
-      </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="M14" s="3">
+        <v>3</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="14"/>
-      <c r="G15" s="3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="12"/>
+      <c r="G15" s="2">
         <v>44859</v>
       </c>
-      <c r="H15" s="4">
-        <v>3</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="L15" s="3">
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="2">
         <v>44876</v>
       </c>
-      <c r="M15" s="4">
-        <v>3</v>
-      </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="M15" s="3">
+        <v>3</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="14"/>
-      <c r="G16" s="3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="12"/>
+      <c r="G16" s="2">
         <v>44861</v>
       </c>
-      <c r="H16" s="4">
-        <v>3</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="L16" s="3">
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="2">
         <v>44879</v>
       </c>
-      <c r="M16" s="4">
-        <v>3</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
+      <c r="M16" s="3">
+        <v>3</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="14"/>
-      <c r="G17" s="3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="12"/>
+      <c r="G17" s="2">
         <v>44862</v>
       </c>
-      <c r="H17" s="4">
-        <v>3</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="L17" s="3">
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="L17" s="2">
         <v>44880</v>
       </c>
-      <c r="M17" s="4">
-        <v>3</v>
-      </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
+      <c r="M17" s="3">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="14"/>
-      <c r="G18" s="3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="12"/>
+      <c r="G18" s="2">
         <v>44863</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <v>4</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="L18" s="3">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="L18" s="2">
         <v>44883</v>
       </c>
-      <c r="M18" s="4">
-        <v>3</v>
-      </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="M18" s="3">
+        <v>3</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="14"/>
-      <c r="G19" s="3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="12"/>
+      <c r="G19" s="2">
         <v>44865</v>
       </c>
-      <c r="H19" s="4">
-        <v>3</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="L19" s="3">
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="L19" s="2">
         <v>44884</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="3">
         <v>4</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="14"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="L20" s="3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="12"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="L20" s="2">
         <v>44886</v>
       </c>
-      <c r="M20" s="4">
-        <v>3</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="M20" s="3">
+        <v>3</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="14"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="L21" s="3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="12"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="L21" s="2">
         <v>44887</v>
       </c>
-      <c r="M21" s="4">
-        <v>3</v>
-      </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
+      <c r="M21" s="3">
+        <v>3</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="14"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="L22" s="3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="12"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="L22" s="2">
         <v>44890</v>
       </c>
-      <c r="M22" s="4">
-        <v>3</v>
-      </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
+      <c r="M22" s="3">
+        <v>3</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="14"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="L23" s="3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="12"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="L23" s="2">
         <v>44893</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="3">
         <v>2</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="14"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="L24" s="3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="12"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="L24" s="2">
         <v>44894</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="3">
         <v>2</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="14"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="L25" s="3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="12"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="L25" s="2">
         <v>44895</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="3">
         <v>6</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4">
         <f>SUM(C10:C25)</f>
         <v>2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <f>SUM(D10:D25)</f>
         <v>2</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f>C26-D26</f>
         <v>0</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="5">
+      <c r="G26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4">
         <f>SUM(H15:H20)</f>
         <v>16</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <f>SUM(I10:I25)</f>
-        <v>6</v>
-      </c>
-      <c r="J26" s="5">
+        <v>9</v>
+      </c>
+      <c r="J26" s="4">
         <f>H26-I26</f>
-        <v>10</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M26" s="5">
+        <v>7</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="4">
         <f>SUM(M10:M25)</f>
         <v>51</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="4">
         <f>SUM(N10:N25)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="4">
         <f>M26-N26</f>
         <v>51</v>
       </c>
-      <c r="Q26" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="R26" s="5">
+      <c r="Q26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R26" s="4">
         <f>SUM(R10:R25)</f>
         <v>14</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="4">
         <f>SUM(S10:S25)</f>
         <v>0</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="4">
         <f>R26-S26</f>
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="1">
         <f>SUM(D26,I26,N26,S26)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1">
         <f>SUM(E26,J26,O26,T26)</f>
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>